<commit_message>
needs further testing, almost ready for full implementation
</commit_message>
<xml_diff>
--- a/google_maps_keywords.xlsx
+++ b/google_maps_keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Desktop\WorkOnword\CitySearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9FBFE0-DAF6-40B6-89A2-47F194809D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE63706-427A-4EA9-A968-B9F45DF21E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6912" yWindow="252" windowWidth="11172" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Country</t>
   </si>
@@ -85,12 +85,6 @@
     <t>San Jose</t>
   </si>
   <si>
-    <t>City1</t>
-  </si>
-  <si>
-    <t>City2</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
@@ -112,13 +106,10 @@
     <t>Queens</t>
   </si>
   <si>
-    <t>South Korea</t>
-  </si>
-  <si>
-    <t>State1</t>
-  </si>
-  <si>
-    <t>State2</t>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Texas</t>
   </si>
 </sst>
 </file>
@@ -407,7 +398,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -520,10 +511,10 @@
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -533,7 +524,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -543,7 +534,7 @@
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -553,7 +544,7 @@
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -563,7 +554,7 @@
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -573,121 +564,76 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="D24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="D26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="5">
     <mergeCell ref="B20:B26"/>
     <mergeCell ref="B27:B30"/>
-    <mergeCell ref="A20:A30"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="B11:B19"/>
-    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="A2:A30"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>